<commit_message>
rename 'spool' to 'dwg'
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="8">
   <si>
     <t>Participant</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Total Time</t>
-  </si>
-  <si>
-    <t>Spool</t>
   </si>
   <si>
     <t>Period</t>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>DWG</t>
   </si>
 </sst>
 </file>
@@ -429,14 +429,14 @@
   <dimension ref="A1:F201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
@@ -444,13 +444,13 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -479,7 +479,7 @@
         <v>429.81</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -499,7 +499,7 @@
         <v>940.52</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -519,7 +519,7 @@
         <v>315.42</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -539,7 +539,7 @@
         <v>153.49</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -559,7 +559,7 @@
         <v>49.67</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -579,7 +579,7 @@
         <v>108.36</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -599,7 +599,7 @@
         <v>96.17</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -619,7 +619,7 @@
         <v>48.59</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -639,7 +639,7 @@
         <v>45.819000000000003</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -659,7 +659,7 @@
         <v>41.021000000000001</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -679,7 +679,7 @@
         <v>719.09</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -699,7 +699,7 @@
         <v>309.82</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -719,7 +719,7 @@
         <v>341.01</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -739,7 +739,7 @@
         <v>102.45</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -759,7 +759,7 @@
         <v>124.99</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -779,7 +779,7 @@
         <v>47.146000000000001</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -799,7 +799,7 @@
         <v>162.72999999999999</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -819,7 +819,7 @@
         <v>128.81</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -839,7 +839,7 @@
         <v>58.502000000000002</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -859,7 +859,7 @@
         <v>30.501999999999999</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -879,7 +879,7 @@
         <v>60.173000000000002</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -899,7 +899,7 @@
         <v>108.35</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -919,7 +919,7 @@
         <v>96.685000000000002</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -939,7 +939,7 @@
         <v>65.617000000000004</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -959,7 +959,7 @@
         <v>46.814</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -979,7 +979,7 @@
         <v>24.908000000000001</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -999,7 +999,7 @@
         <v>92.153000000000006</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1019,7 +1019,7 @@
         <v>86.91</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1039,7 +1039,7 @@
         <v>91.222999999999999</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1059,7 +1059,7 @@
         <v>18.521000000000001</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1071,6 +1071,15 @@
       </c>
       <c r="C32" s="3">
         <v>1</v>
+      </c>
+      <c r="D32" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="E32" s="5">
+        <v>429.81</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>